<commit_message>
now tracks player and game definition creations in universal analytics.
</commit_message>
<xml_diff>
--- a/SEO_Dashboards/SEO_Dashboard.xlsx
+++ b/SEO_Dashboards/SEO_Dashboard.xlsx
@@ -182,7 +182,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="177">
   <si>
     <t>Current URL</t>
   </si>
@@ -743,6 +743,108 @@
   </si>
   <si>
     <t>https://nerdscorekeeper.azurewebsites.net</t>
+  </si>
+  <si>
+    <t>board game</t>
+  </si>
+  <si>
+    <t>board games</t>
+  </si>
+  <si>
+    <t>board game tracking</t>
+  </si>
+  <si>
+    <t>board game statistics</t>
+  </si>
+  <si>
+    <t>game statistics</t>
+  </si>
+  <si>
+    <t>board gaming</t>
+  </si>
+  <si>
+    <t>gaming statistics</t>
+  </si>
+  <si>
+    <t>track board game wins</t>
+  </si>
+  <si>
+    <t>track board game statistics</t>
+  </si>
+  <si>
+    <t>track who wins board games</t>
+  </si>
+  <si>
+    <t>game tracker</t>
+  </si>
+  <si>
+    <t>gaming tracker</t>
+  </si>
+  <si>
+    <t>game tracking</t>
+  </si>
+  <si>
+    <t>nemestats</t>
+  </si>
+  <si>
+    <t>fun board game statistics</t>
+  </si>
+  <si>
+    <t>fun board game tracker</t>
+  </si>
+  <si>
+    <t>free board game tracker</t>
+  </si>
+  <si>
+    <t>board game tracking free</t>
+  </si>
+  <si>
+    <t>board game statistics free</t>
+  </si>
+  <si>
+    <t>game statistics free</t>
+  </si>
+  <si>
+    <t>track win/loss ratio</t>
+  </si>
+  <si>
+    <t>free tracking of board games</t>
+  </si>
+  <si>
+    <t>record games</t>
+  </si>
+  <si>
+    <t>record board games</t>
+  </si>
+  <si>
+    <t>record board games free</t>
+  </si>
+  <si>
+    <t>board game tracking app</t>
+  </si>
+  <si>
+    <t>free board game tracking app</t>
+  </si>
+  <si>
+    <t>board game tracking online</t>
+  </si>
+  <si>
+    <t>free online board game</t>
+  </si>
+  <si>
+    <t>board games online free</t>
+  </si>
+  <si>
+    <t>board game online free friends</t>
+  </si>
+  <si>
+    <t>friends board gaming</t>
+  </si>
+  <si>
+    <t>board game online tracking free</t>
+  </si>
+  <si>
+    <t>board game track friends free</t>
   </si>
 </sst>
 </file>
@@ -3704,107 +3806,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>3714750</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Rectangle 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="57150" y="1200150"/>
-          <a:ext cx="3657600" cy="914400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="B92025"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-            <a:prstClr val="black">
-              <a:alpha val="40000"/>
-            </a:prstClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Start with your own brain. List all</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> of the terms you'd like your site to rank for.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100" b="1" i="1" baseline="0">
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" i="1" baseline="0">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Shoot for at least 50.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="0" i="1">
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
       <xdr:row>3</xdr:row>
@@ -4145,15 +4146,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>57148</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>266698</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2657475</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:colOff>2600325</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4162,7 +4163,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="57150" y="1885948"/>
+          <a:off x="0" y="3009898"/>
           <a:ext cx="2600325" cy="2219327"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -8190,8 +8191,8 @@
   <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="A1:D12"/>
+      <pane ySplit="3" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.42578125" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8230,106 +8231,174 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
+      <c r="A4" s="17" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
+      <c r="A5" s="18" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
+      <c r="A6" s="18" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
+      <c r="A7" s="18" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
+      <c r="A8" s="18" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
+      <c r="A9" s="18" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="10" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
+      <c r="A10" s="18" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
+      <c r="A11" s="18" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
+      <c r="A12" s="18" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
+      <c r="A13" s="18" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="14" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
+      <c r="A14" s="18" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
+      <c r="A15" s="18" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="16" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
+      <c r="A16" s="18" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="17" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
+      <c r="A17" s="18" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="18" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
+      <c r="A18" s="18" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="19" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
+      <c r="A19" s="18" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="20" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
+      <c r="A20" s="18" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="21" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
+      <c r="A21" s="18" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="22" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
+      <c r="A22" s="18" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="23" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
+      <c r="A23" s="18" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="24" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
+      <c r="A24" s="18" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="25" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
+      <c r="A25" s="18" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="26" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
+      <c r="A26" s="18" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="27" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
+      <c r="A27" s="18" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="28" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="18"/>
+      <c r="A28" s="18" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="29" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
+      <c r="A29" s="18" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="30" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
+      <c r="A30" s="18" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="31" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
+      <c r="A31" s="18" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="32" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
+      <c r="A32" s="18" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="33" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="18"/>
+      <c r="A33" s="18" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="34" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
+      <c r="A34" s="18" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="35" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="18"/>
+      <c r="A35" s="18" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="36" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="18"/>
+      <c r="A36" s="18" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="37" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="18"/>
+      <c r="A37" s="18" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="38" spans="1:1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="18"/>

</xml_diff>